<commit_message>
Envio de correo electronico version 1
</commit_message>
<xml_diff>
--- a/topdown/topdown FCEC.xlsx
+++ b/topdown/topdown FCEC.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840" activeTab="3"/>
+    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Proyecto" sheetId="1" r:id="rId1"/>
-    <sheet name="email" sheetId="2" r:id="rId2"/>
-    <sheet name="GIT" sheetId="3" r:id="rId3"/>
-    <sheet name="pendientes" sheetId="4" r:id="rId4"/>
+    <sheet name="Tareas pendientes" sheetId="5" r:id="rId1"/>
+    <sheet name="weblografia" sheetId="8" r:id="rId2"/>
+    <sheet name="Proyecto" sheetId="1" r:id="rId3"/>
+    <sheet name="email" sheetId="2" r:id="rId4"/>
+    <sheet name="GIT" sheetId="3" r:id="rId5"/>
+    <sheet name="pendientes" sheetId="4" r:id="rId6"/>
+    <sheet name="checkbox" sheetId="6" r:id="rId7"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="193">
   <si>
     <t>NOMBRE DEL PROYECTO:</t>
   </si>
@@ -230,13 +234,607 @@
   </si>
   <si>
     <t>Revisar configuracion de BOOTSTRAP</t>
+  </si>
+  <si>
+    <t>menvios</t>
+  </si>
+  <si>
+    <t>Tarea o Error pendiente de revisión</t>
+  </si>
+  <si>
+    <t>No muestra la consistencia.</t>
+  </si>
+  <si>
+    <t>No muestra el valor del campo whatsapp. Siempre muestra TRUE.</t>
+  </si>
+  <si>
+    <t>PROCESO</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>DataUsers</t>
+  </si>
+  <si>
+    <t>Controlador</t>
+  </si>
+  <si>
+    <t>DatausersController.php</t>
+  </si>
+  <si>
+    <t>GrupoCursosController.php</t>
+  </si>
+  <si>
+    <t>Model (sólo si se modifica)</t>
+  </si>
+  <si>
+    <t>Migration (sólo si se modifica)</t>
+  </si>
+  <si>
+    <t>Modificar orden</t>
+  </si>
+  <si>
+    <t>Crear Grupo</t>
+  </si>
+  <si>
+    <t>¿Es necesario?</t>
+  </si>
+  <si>
+    <t>Vista (en rojo los que faltan crear)</t>
+  </si>
+  <si>
+    <t>EnviosController.php</t>
+  </si>
+  <si>
+    <t>Menvios</t>
+  </si>
+  <si>
+    <t>add_menvios_table</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Mostrar los correos enviados</t>
+  </si>
+  <si>
+    <t>add_denvios_table</t>
+  </si>
+  <si>
+    <t>Denvios</t>
+  </si>
+  <si>
+    <t>Crear migration y model ( agregar campo TABLENAME - que debe tener el campo SW_RPTA)</t>
+  </si>
+  <si>
+    <t>Crea los requerimientos (agregar campo TX_NEED - texto del correo)</t>
+  </si>
+  <si>
+    <t>Función de recorrido de las tablas previstas en Menvios poniendo check en SW_RPTA y contándolos.</t>
+  </si>
+  <si>
+    <t>Envía los correos electrónicos del requerimiento.</t>
+  </si>
+  <si>
+    <t>Auth/login.blade.php</t>
+  </si>
+  <si>
+    <t>admin/datausers/edit.blade.php</t>
+  </si>
+  <si>
+    <t>admin/grupoCursos/create.blade.php</t>
+  </si>
+  <si>
+    <t>admin/grupoCursos/orden.blade.php</t>
+  </si>
+  <si>
+    <t>admin/envios/index.blade.php</t>
+  </si>
+  <si>
+    <t>admin/envios/create.blade.php</t>
+  </si>
+  <si>
+    <t>REALIZADO</t>
+  </si>
+  <si>
+    <t>Configurar el SEARCH en el Controller</t>
+  </si>
+  <si>
+    <t>tfcia_rptas</t>
+  </si>
+  <si>
+    <t>recontar_envios</t>
+  </si>
+  <si>
+    <t>recontar_rptas</t>
+  </si>
+  <si>
+    <t>denvios</t>
+  </si>
+  <si>
+    <t>Agrega los docentes a comunicar.</t>
+  </si>
+  <si>
+    <t>dcreate/dstore</t>
+  </si>
+  <si>
+    <t>{{ Form::hidden('whatsapp', 0) }}</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;</t>
+  </si>
+  <si>
+    <t>@if($datauser-&gt;whatsapp == 1)</t>
+  </si>
+  <si>
+    <t>{!! Form::checkbox('whatsapp', 1, true, ['class'=&gt;'checkbox', 'onclick' =&gt; 'javascript:evento(this);'] ) !!}</t>
+  </si>
+  <si>
+    <t>@else</t>
+  </si>
+  <si>
+    <t>{!! Form::checkbox('whatsapp', 0, false, ['class'=&gt;'checkbox', 'onclick' =&gt; 'javascript:evento(this);'] ) !!}</t>
+  </si>
+  <si>
+    <t>@endif</t>
+  </si>
+  <si>
+    <t>&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>@section('js')</t>
+  </si>
+  <si>
+    <t>function evento($obj){</t>
+  </si>
+  <si>
+    <t>//console.log($obj);</t>
+  </si>
+  <si>
+    <t>if($obj.checked)</t>
+  </si>
+  <si>
+    <t>$obj.value = 1;</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>$obj.value = 0;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>&lt;script type="text/javascript"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>@endsection</t>
+  </si>
+  <si>
+    <t>Tratamiento de checkbox</t>
+  </si>
+  <si>
+    <t>Asignar valor 0 a la variable</t>
+  </si>
+  <si>
+    <t>Segun el valor de la tabla</t>
+  </si>
+  <si>
+    <t>Agregar funcion evento 'onclick'</t>
+  </si>
+  <si>
+    <t>Seccion js</t>
+  </si>
+  <si>
+    <t>Funcion 'evento'</t>
+  </si>
+  <si>
+    <t>&lt;!-- INICIO DEL BUSCADOR  --&gt;</t>
+  </si>
+  <si>
+    <t>{!! Form::open(['route' =&gt; 'admin.menvios.dshow', 'method'=&gt;'GET', 'class'=&gt;'navbar-form pull-right']) !!}</t>
+  </si>
+  <si>
+    <t>&lt;div class="input-group"&gt;</t>
+  </si>
+  <si>
+    <t>{!! Form::text('tipo', null, ['class'=&gt;'form-control', 'placeholder'=&gt;'Filtrar por nombre ...', 'aria-describedby'=&gt;'search']) !!}</t>
+  </si>
+  <si>
+    <t>&lt;span class="input-group-addon" id='search'&gt;&lt;span class="glyphicon glyphicon-search" "aria-hidden"="true"&gt;&lt;/span&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>{!! Form::close() !!}</t>
+  </si>
+  <si>
+    <t>&lt;!-- FIN DEL BUSCADOR --&gt;</t>
+  </si>
+  <si>
+    <t>$message-&gt;subject($subject);</t>
+  </si>
+  <si>
+    <t>$message-&gt;priority($level);</t>
+  </si>
+  <si>
+    <t>// Attach a file from a raw $data string...</t>
+  </si>
+  <si>
+    <t>// Get the underlying SwiftMailer message instance...</t>
+  </si>
+  <si>
+    <t>$message-&gt;getSwiftMessage();</t>
+  </si>
+  <si>
+    <r>
+      <t>Here is a list of the available methods on the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>$message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> message builder instance:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;from($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;sender($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;to($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;cc($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;bcc($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;replyTo($address, $name = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;attach($pathToFile, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> $options = []);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$message-&gt;attachData($data, $name, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> $options = []);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Nota:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> La instancia del mensaje pasada al Closure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.9"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Mail::send</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> extiende de la clase mensaje de SwiftMailer, permitiéndote llamar a cualquier método en esa clase para construir tus mensajes de correo electrónico.</t>
+    </r>
+  </si>
+  <si>
+    <t>http://laraveles.com/docs/5.1/mail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mail::send('emails.welcome', $data, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ($message) { </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$message-&gt;from('us@example.com', 'Laravel'); </t>
+  </si>
+  <si>
+    <t>$message-&gt;to('foo@example.com')-&gt;cc('bar@example.com');</t>
+  </si>
+  <si>
+    <t>});</t>
+  </si>
+  <si>
+    <t>https://aprendible.com/cursos</t>
+  </si>
+  <si>
+    <t>https://www.google.com/settings/security/lesssecureapps</t>
+  </si>
+  <si>
+    <t>desactivar seguridad en gmail</t>
+  </si>
+  <si>
+    <t>create/store</t>
+  </si>
+  <si>
+    <t>admin/envios/list.blade.php</t>
+  </si>
+  <si>
+    <t>admin/envios/email.blade.php</t>
+  </si>
+  <si>
+    <t>MenviosController.php</t>
+  </si>
+  <si>
+    <r>
+      <t>show/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PDF</t>
+    </r>
+  </si>
+  <si>
+    <t>dupdate</t>
+  </si>
+  <si>
+    <t>Funciones private</t>
+  </si>
+  <si>
+    <t>dmarkall</t>
+  </si>
+  <si>
+    <t>dunmarkall</t>
+  </si>
+  <si>
+    <t>ACCESO</t>
+  </si>
+  <si>
+    <t>RESPONSABLES</t>
+  </si>
+  <si>
+    <t>CORREOS</t>
+  </si>
+  <si>
+    <t>Falta definir correos por tipo</t>
+  </si>
+  <si>
+    <t>Falta revisar QUEUES (Trabajos en cola)</t>
+  </si>
+  <si>
+    <t>us$ 75.00</t>
+  </si>
+  <si>
+    <t>laraveles.com</t>
+  </si>
+  <si>
+    <t>https://laravel.com/docs/5.3</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
+  </si>
+  <si>
+    <t>https://laravelcollective.com/docs/5.0/html</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/components/</t>
+  </si>
+  <si>
+    <t>Bootstrap - componentes</t>
+  </si>
+  <si>
+    <t>https://styde.net</t>
+  </si>
+  <si>
+    <t>Foro</t>
+  </si>
+  <si>
+    <t>https://secure.php.net/manual/es/index.php</t>
+  </si>
+  <si>
+    <t>PHP español</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +865,74 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,7 +942,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -284,12 +950,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -305,6 +1051,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -608,10 +1418,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.90625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.1796875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.90625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D5" s="31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="C16" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="22"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E27" s="33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E28" s="33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,13 +1759,18 @@
     <col min="4" max="4" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.08984375" style="2" customWidth="1"/>
     <col min="8" max="8" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,341 +1778,492 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5" s="2"/>
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6" s="2"/>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" s="2"/>
+      <c r="O7" s="13"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="H8" s="14"/>
+      <c r="J8" s="13"/>
+      <c r="L8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="J9" s="13"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="J10" s="13"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="J11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="J12" s="13"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="J13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="J14" s="13"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="13"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="J15" s="13"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D16" s="14"/>
+      <c r="F16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="J16" s="13"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="14"/>
+      <c r="F17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="J17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="13"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D18" s="14"/>
+      <c r="F18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="J18" s="13"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D19" s="14"/>
+      <c r="F19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="J19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="13"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D20" s="14"/>
+      <c r="F20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="J20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="13"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L21" s="14"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L22" s="14"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="13"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D23" s="14"/>
+      <c r="F23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="J23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="13"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="17"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="17"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="H3:J3"/>
+    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -978,17 +2271,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -996,7 +2289,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>45</v>
       </c>
@@ -1004,22 +2297,239 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A14" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="22"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="22"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="23"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A37:H37"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -1150,11 +2660,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1173,4 +2683,213 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <f>+B11+B12</f>
+        <v>521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de correo electronico version 2
</commit_message>
<xml_diff>
--- a/topdown/topdown FCEC.xlsx
+++ b/topdown/topdown FCEC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840" activeTab="1"/>
+    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas pendientes" sheetId="5" r:id="rId1"/>
@@ -16,12 +16,15 @@
     <sheet name="checkbox" sheetId="6" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="7" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tareas pendientes'!$A$1:$I$33</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="216">
   <si>
     <t>NOMBRE DEL PROYECTO:</t>
   </si>
@@ -245,9 +248,6 @@
     <t>No muestra la consistencia.</t>
   </si>
   <si>
-    <t>No muestra el valor del campo whatsapp. Siempre muestra TRUE.</t>
-  </si>
-  <si>
     <t>PROCESO</t>
   </si>
   <si>
@@ -272,9 +272,6 @@
     <t>Migration (sólo si se modifica)</t>
   </si>
   <si>
-    <t>Modificar orden</t>
-  </si>
-  <si>
     <t>Crear Grupo</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>admin/grupoCursos/create.blade.php</t>
   </si>
   <si>
-    <t>admin/grupoCursos/orden.blade.php</t>
-  </si>
-  <si>
     <t>admin/envios/index.blade.php</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
   </si>
   <si>
     <t>REALIZADO</t>
-  </si>
-  <si>
-    <t>Configurar el SEARCH en el Controller</t>
   </si>
   <si>
     <t>tfcia_rptas</t>
@@ -773,9 +764,6 @@
     <t>dupdate</t>
   </si>
   <si>
-    <t>Funciones private</t>
-  </si>
-  <si>
     <t>dmarkall</t>
   </si>
   <si>
@@ -785,9 +773,6 @@
     <t>ACCESO</t>
   </si>
   <si>
-    <t>RESPONSABLES</t>
-  </si>
-  <si>
     <t>CORREOS</t>
   </si>
   <si>
@@ -828,6 +813,93 @@
   </si>
   <si>
     <t>PHP español</t>
+  </si>
+  <si>
+    <t>Editar el registro del maestro de envios</t>
+  </si>
+  <si>
+    <t>agregar campo sw_envio en menvios</t>
+  </si>
+  <si>
+    <t>Funciones private ???</t>
+  </si>
+  <si>
+    <t>Documentos en PDF</t>
+  </si>
+  <si>
+    <t>savePDF</t>
+  </si>
+  <si>
+    <t>admin/datausers/upPDF.blade.php</t>
+  </si>
+  <si>
+    <t>Ingreso de documentos en PDF.</t>
+  </si>
+  <si>
+    <t>nueva tabla</t>
+  </si>
+  <si>
+    <t>DataPDF</t>
+  </si>
+  <si>
+    <t>SW_PDTE</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>UP PDF</t>
+  </si>
+  <si>
+    <t>https://styde.net/variables-de-entorno-en-laravel/</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>UsersController.php</t>
+  </si>
+  <si>
+    <t>Crear accesos con tabla</t>
+  </si>
+  <si>
+    <t>edit/update</t>
+  </si>
+  <si>
+    <t>Modificar cursos del grupo</t>
+  </si>
+  <si>
+    <t>Modificar prioridad de docentes</t>
+  </si>
+  <si>
+    <t>admin/grupoCursos/prioridad.blade.php</t>
+  </si>
+  <si>
+    <t>prioridad/update_prioridad</t>
+  </si>
+  <si>
+    <t>GRUPOS</t>
+  </si>
+  <si>
+    <t>Modificar descripcion del grupo</t>
+  </si>
+  <si>
+    <t>GruposController.php</t>
+  </si>
+  <si>
+    <t>admin/grupos/edit.blade.php</t>
+  </si>
+  <si>
+    <t>{{dd($chunk)}};</t>
+  </si>
+  <si>
+    <t>{{$chunk = $dcursos-&gt;splice($xobj-1)}};</t>
+  </si>
+  <si>
+    <t>{{dd($plucked)}};</t>
+  </si>
+  <si>
+    <t>{{$plucked = $cursos-&gt;pluck('id')}};</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1080,21 +1152,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1115,6 +1172,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1418,254 +1496,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.90625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.81640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.1796875" style="33" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="26.08984375" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.90625" style="31"/>
+    <col min="1" max="1" width="8.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.1796875" style="28" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="26.08984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" style="26" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="E3" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="10" t="s">
+      <c r="E5" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="10" t="s">
+      <c r="H17" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="D18" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D20" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D21" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D22" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="D23" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D24" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D25" s="22" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D5" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="34" t="s">
+      <c r="E25" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D26" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D27" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D28" s="22"/>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C29" s="22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="C16" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="33" t="s">
+      <c r="D29" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C30" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="22" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C31" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="27" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="22"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E27" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E28" s="33" t="s">
-        <v>181</v>
-      </c>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I33">
+    <filterColumn colId="2" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1674,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1686,56 +1913,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
-        <v>165</v>
+      <c r="A1" s="32" t="s">
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1782,24 +2014,24 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="9"/>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="29"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1963,7 +2195,7 @@
         <v>71</v>
       </c>
       <c r="O8" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -2248,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2257,10 +2489,10 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -2309,28 +2541,28 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -2338,7 +2570,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -2356,7 +2588,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -2366,7 +2598,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -2376,7 +2608,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -2386,7 +2618,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -2396,7 +2628,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2406,7 +2638,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -2416,7 +2648,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -2426,7 +2658,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -2436,7 +2668,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -2454,7 +2686,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -2464,7 +2696,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -2482,7 +2714,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2492,7 +2724,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -2509,16 +2741,16 @@
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
+      <c r="A37" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2533,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2700,120 +2932,120 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2825,52 +3057,52 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2889,6 +3121,26 @@
         <v>521</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Envio de correo electronico version 3
</commit_message>
<xml_diff>
--- a/topdown/topdown FCEC.xlsx
+++ b/topdown/topdown FCEC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840"/>
+    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas pendientes" sheetId="5" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="pendientes" sheetId="4" r:id="rId6"/>
     <sheet name="checkbox" sheetId="6" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="7" r:id="rId8"/>
+    <sheet name="Rutas View" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tareas pendientes'!$A$1:$I$33</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="224">
   <si>
     <t>NOMBRE DEL PROYECTO:</t>
   </si>
@@ -900,6 +901,30 @@
   </si>
   <si>
     <t>{{$plucked = $cursos-&gt;pluck('id')}};</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>indice</t>
+  </si>
+  <si>
+    <t>vistas</t>
+  </si>
+  <si>
+    <t>edicion</t>
+  </si>
+  <si>
+    <t>todo</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -3144,4 +3169,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de Correos con Gmail
</commit_message>
<xml_diff>
--- a/topdown/topdown FCEC.xlsx
+++ b/topdown/topdown FCEC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840" activeTab="7"/>
+    <workbookView xWindow="320" yWindow="120" windowWidth="17700" windowHeight="4840"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas pendientes" sheetId="5" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="7" r:id="rId7"/>
     <sheet name="Routing" sheetId="9" r:id="rId8"/>
     <sheet name="routeList" sheetId="10" r:id="rId9"/>
+    <sheet name="Hoja2" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tareas pendientes'!$A$1:$I$36</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="392">
   <si>
     <t>NOMBRE DEL PROYECTO:</t>
   </si>
@@ -1197,12 +1198,6 @@
     <t>|        | POST      | register                             |                             | App\Http\Controllers\Auth\AuthController@register               | web,web</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -1242,9 +1237,6 @@
     <t>Revisar plugins</t>
   </si>
   <si>
-    <t>Crear accesos con tabla individual</t>
-  </si>
-  <si>
     <t>DISPONIBILIDAD</t>
   </si>
   <si>
@@ -1303,6 +1295,159 @@
   </si>
   <si>
     <t>Ruteo en Responsables</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>CONTROLLER</t>
+  </si>
+  <si>
+    <t>uses</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>ROUTE</t>
+  </si>
+  <si>
+    <t>//devuelve el nombre del rol del usuario según el número</t>
+  </si>
+  <si>
+    <t>if(!function_exists('getRole'))</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> function getRole($role)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> switch ($role) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case '00':</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Invitado.";</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case '01':</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Administrativo.";</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case '02':</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Docente.";</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case '03':</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Responsable.";</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> break; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case '09':</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Master.";</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> default:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/*ruta con el prefijo home que comprueba primero si </t>
+  </si>
+  <si>
+    <t>//existe la sesión, si es así comprueba el rol del usuario</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/admin: 3</t>
+  </si>
+  <si>
+    <t>/editor: 2</t>
+  </si>
+  <si>
+    <t>/suscriptor: 1</t>
+  </si>
+  <si>
+    <t>/invitado: 0</t>
+  </si>
+  <si>
+    <t>*/</t>
+  </si>
+  <si>
+    <t>Route::group(array('prefix' =&gt; 'admin','before' =&gt; 'auth'), function()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //http://localhost/roles_users_laravel/public/home/admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //sólo pueden acceder usuarios con role_id 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Route::get('admin',array("before" =&gt; "roles:'09',admin", function()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Como mínimo tu role debe ser master, tu eres " . getRole(Auth::user()-&gt;type);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> }));</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //http://localhost/roles_users_laravel/public/home/new_post</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //sólo pueden acceder usuarios con role_id 2 y 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Route::get('new_post',array("before" =&gt; "roles:03-09,admin", function()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Como mínimo tu role debe ser responsable, tu eres " . getRole(Auth::user()-&gt;type);</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //http://localhost/roles_users_laravel/public/home/show_reply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //sólo pueden acceder usuarios con role_id 1, 2 y 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Route::get('show_reply',array("before" =&gt; "roles:02-03-09,admin", function()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return "Como mínimo tu role debe ser docente, tu eres " . getRole(Auth::user()-&gt;type);</t>
+  </si>
+  <si>
+    <t>Dcurso</t>
+  </si>
+  <si>
+    <t>Cuatro tipos de usuarios</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1439,6 +1584,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1536,7 +1687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1606,21 +1757,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1631,12 +1767,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1646,20 +1776,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1679,9 +1800,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1694,9 +1812,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2002,8 +2163,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2027,10 +2188,10 @@
       <c r="B1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="35"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="10" t="s">
         <v>84</v>
       </c>
@@ -2066,33 +2227,25 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
-        <v>185</v>
-      </c>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
-        <v>185</v>
-      </c>
+      <c r="F4" s="31" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" s="26" t="s">
         <v>187</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>323</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>182</v>
-      </c>
+      <c r="F5" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="26" t="s">
@@ -2211,7 +2364,7 @@
         <v>192</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35"/>
@@ -2404,24 +2557,21 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="26" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="32" t="s">
-        <v>185</v>
-      </c>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2438,6 +2588,361 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:A71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2480,24 +2985,24 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="9"/>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="38"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -2946,7 +3451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2957,7 +3462,7 @@
       <c r="B1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="69" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3207,16 +3712,16 @@
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3617,10 +4122,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3633,12 +4138,15 @@
     <col min="6" max="6" width="6.1796875" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" style="28" customWidth="1"/>
     <col min="8" max="8" width="12.7265625" style="26" customWidth="1"/>
-    <col min="9" max="11" width="10.90625" style="26"/>
-    <col min="12" max="12" width="11.1796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.90625" style="26"/>
+    <col min="9" max="10" width="10.90625" style="26"/>
+    <col min="11" max="11" width="6.08984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.90625" style="26"/>
+    <col min="13" max="14" width="4.7265625" style="26" customWidth="1"/>
+    <col min="15" max="15" width="80.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.90625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="26" t="s">
         <v>202</v>
       </c>
@@ -3646,12 +4154,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="26" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="26" t="s">
         <v>203</v>
       </c>
@@ -3659,7 +4167,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="26" t="s">
         <v>204</v>
       </c>
@@ -3667,7 +4175,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="26" t="s">
         <v>205</v>
       </c>
@@ -3675,330 +4183,517 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="40" t="s">
-        <v>321</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-    </row>
-    <row r="10" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="40"/>
-      <c r="C10" s="49" t="s">
+    <row r="9" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="35"/>
+      <c r="C10" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66" t="s">
+        <v>335</v>
+      </c>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="35"/>
+      <c r="L10" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="44" t="s">
-        <v>338</v>
-      </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-    </row>
-    <row r="11" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="C11" s="48" t="s">
+      <c r="F11" s="50" t="s">
+        <v>329</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="51" t="s">
         <v>337</v>
       </c>
-      <c r="D11" s="59" t="s">
-        <v>341</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>342</v>
-      </c>
-      <c r="F11" s="61" t="s">
-        <v>332</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>333</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>331</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>308</v>
-      </c>
-      <c r="L11" s="26" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="52" t="str">
+        <f>LOWER(F12)&amp;"s"</f>
+        <v>dcursos</v>
+      </c>
+      <c r="D12" s="52" t="str">
+        <f>+C12</f>
+        <v>dcursos</v>
+      </c>
+      <c r="E12" s="45"/>
+      <c r="F12" s="52" t="s">
+        <v>390</v>
+      </c>
+      <c r="G12" s="26"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+    </row>
+    <row r="13" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="62" t="s">
-        <v>340</v>
-      </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="63" t="str">
-        <f>LOWER(F12)&amp;"s"</f>
-        <v>users</v>
-      </c>
-      <c r="D12" s="63" t="str">
+      <c r="C13" s="53" t="str">
         <f>+C12</f>
-        <v>users</v>
-      </c>
-      <c r="E12" s="55"/>
-      <c r="F12" s="63" t="s">
-        <v>310</v>
-      </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-    </row>
-    <row r="13" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="C13" s="64" t="str">
-        <f>+C12</f>
-        <v>users</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="64" t="str">
+        <v>dcursos</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="53" t="str">
         <f>+F12</f>
-        <v>User</v>
+        <v>Dcurso</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>329</v>
+        <v>313</v>
+      </c>
+      <c r="J13" s="26" t="str">
+        <f>+"admin."&amp;$D$12</f>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L13" s="26" t="str">
+        <f t="shared" ref="L13:L19" si="0">+"'"&amp;C13&amp;IF(LEN(D13)&gt;0,"/{"&amp;D13&amp;"}","")&amp;IF(LEN(E13)&gt;0,"/"&amp;E13,"")&amp;"'"</f>
+        <v>'dcursos'</v>
       </c>
       <c r="M13" s="26" t="str">
-        <f>+"Route::"&amp;B13&amp;"('"&amp;C13&amp;IF(LEN(D13)&gt;0,"/{"&amp;D13&amp;"}"&amp;IF(LEN(E13)&gt;0,"/"&amp;E13,""),"")&amp;"',['uses' =&gt; '"&amp;F13&amp;"sController@"&amp;G13&amp;"','as'=&gt; '"&amp;J13&amp;"."&amp;G13&amp;"']);"</f>
-        <v>Route::get('users',['uses' =&gt; 'UsersController@index','as'=&gt; 'admin.users.index']);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+        <f>+"'uses'=&gt;'"&amp;F13&amp;"sController@"&amp;G13&amp;"'"</f>
+        <v>'uses'=&gt;'DcursosController@index'</v>
+      </c>
+      <c r="N13" s="26" t="str">
+        <f>+"'as'=&gt;'"&amp;J13&amp;"."&amp;G13&amp;"'"</f>
+        <v>'as'=&gt;'admin.dcursos.index'</v>
+      </c>
+      <c r="O13" s="57" t="str">
+        <f t="shared" ref="O13:O19" si="1">+"Route::"&amp;B13&amp;"("&amp;L13&amp;",["&amp;M13&amp;","&amp;N13&amp;"]);"</f>
+        <v>Route::get('dcursos',['uses'=&gt;'DcursosController@index','as'=&gt;'admin.dcursos.index']);</v>
+      </c>
+      <c r="P13" s="26" t="str">
+        <f t="shared" ref="P13:P19" si="2">+"Route::"&amp;B13&amp;"('"&amp;C13&amp;IF(LEN(D13)&gt;0,"/{"&amp;D13&amp;"}"&amp;IF(LEN(E13)&gt;0,"/"&amp;E13,""),"")&amp;"',['uses' =&gt; '"&amp;F13&amp;"sController@"&amp;G13&amp;"','as'=&gt; '"&amp;J13&amp;"."&amp;G13&amp;"']);"</f>
+        <v>Route::get('dcursos',['uses' =&gt; 'DcursosController@index','as'=&gt; 'admin.dcursos.index']);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="C14" s="64" t="str">
-        <f t="shared" ref="C14:C19" si="0">+C13</f>
-        <v>users</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="64" t="str">
-        <f>+F13</f>
-        <v>User</v>
+        <v>309</v>
+      </c>
+      <c r="C14" s="53" t="str">
+        <f>+C15</f>
+        <v>dcursos</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="53" t="str">
+        <f>+G14</f>
+        <v>create</v>
+      </c>
+      <c r="F14" s="53" t="str">
+        <f>+F15</f>
+        <v>Dcurso</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>329</v>
+        <v>21</v>
+      </c>
+      <c r="H14" s="28"/>
+      <c r="J14" s="26" t="str">
+        <f>+J13</f>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L14" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>'dcursos/create'</v>
       </c>
       <c r="M14" s="26" t="str">
-        <f t="shared" ref="M14:M19" si="1">+"Route::"&amp;B14&amp;"('"&amp;C14&amp;IF(LEN(D14)&gt;0,"/{"&amp;D14&amp;"}"&amp;IF(LEN(E14)&gt;0,"/"&amp;E14,""),"")&amp;"',['uses' =&gt; '"&amp;F14&amp;"sController@"&amp;G14&amp;"','as'=&gt; '"&amp;J14&amp;"."&amp;G14&amp;"']);"</f>
-        <v>Route::post('users',['uses' =&gt; 'UsersController@store','as'=&gt; 'admin.users.store']);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+        <f t="shared" ref="M14:M19" si="3">+"'uses'=&gt;'"&amp;F14&amp;"sController@"&amp;G14&amp;"'"</f>
+        <v>'uses'=&gt;'DcursosController@create'</v>
+      </c>
+      <c r="N14" s="26" t="str">
+        <f t="shared" ref="N14:N19" si="4">+"'as'=&gt;'"&amp;J14&amp;"."&amp;G14&amp;"'"</f>
+        <v>'as'=&gt;'admin.dcursos.create'</v>
+      </c>
+      <c r="O14" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>Route::get('dcursos/create',['uses'=&gt;'DcursosController@create','as'=&gt;'admin.dcursos.create']);</v>
+      </c>
+      <c r="P14" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::get('dcursos',['uses' =&gt; 'DcursosController@create','as'=&gt; 'admin.dcursos.create']);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="C15" s="64" t="str">
+      <c r="C15" s="53" t="str">
+        <f>+C13</f>
+        <v>dcursos</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="53" t="str">
+        <f>+F13</f>
+        <v>Dcurso</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="J15" s="26" t="str">
+        <f t="shared" ref="J15:J19" si="5">+J14</f>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L15" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>users</v>
-      </c>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="64" t="str">
-        <f t="shared" ref="F15:F19" si="2">+F14</f>
-        <v>User</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="28"/>
-      <c r="J15" s="26" t="s">
-        <v>329</v>
+        <v>'dcursos'</v>
       </c>
       <c r="M15" s="26" t="str">
+        <f>+"'uses'=&gt;'"&amp;F15&amp;"sController@"&amp;G15&amp;"'"</f>
+        <v>'uses'=&gt;'DcursosController@store'</v>
+      </c>
+      <c r="N15" s="26" t="str">
+        <f>+"'as'=&gt;'"&amp;J15&amp;"."&amp;G15&amp;"'"</f>
+        <v>'as'=&gt;'admin.dcursos.store'</v>
+      </c>
+      <c r="O15" s="57" t="str">
         <f t="shared" si="1"/>
-        <v>Route::get('users',['uses' =&gt; 'UsersController@create','as'=&gt; 'admin.users.create']);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>Route::post('dcursos',['uses'=&gt;'DcursosController@store','as'=&gt;'admin.dcursos.store']);</v>
+      </c>
+      <c r="P15" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::post('dcursos',['uses' =&gt; 'DcursosController@store','as'=&gt; 'admin.dcursos.store']);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="C16" s="64" t="str">
+        <v>324</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>309</v>
+      </c>
+      <c r="C16" s="53" t="str">
+        <f>+C14</f>
+        <v>dcursos</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="53" t="str">
+        <f>+F14</f>
+        <v>Dcurso</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="J16" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L16" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>users</v>
-      </c>
-      <c r="D16" s="64" t="str">
+        <v>'dcursos/{users}/edit'</v>
+      </c>
+      <c r="M16" s="26" t="str">
+        <f t="shared" si="3"/>
+        <v>'uses'=&gt;'DcursosController@edit'</v>
+      </c>
+      <c r="N16" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v>'as'=&gt;'admin.dcursos.edit'</v>
+      </c>
+      <c r="O16" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>Route::get('dcursos/{users}/edit',['uses'=&gt;'DcursosController@edit','as'=&gt;'admin.dcursos.edit']);</v>
+      </c>
+      <c r="P16" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::get('dcursos/{users}/edit',['uses' =&gt; 'DcursosController@edit','as'=&gt; 'admin.dcursos.edit']);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C17" s="53" t="str">
+        <f t="shared" ref="C17:C19" si="6">+C16</f>
+        <v>dcursos</v>
+      </c>
+      <c r="D17" s="53" t="str">
         <f>+D12</f>
-        <v>users</v>
-      </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v>User</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="H16" s="28" t="s">
+        <v>dcursos</v>
+      </c>
+      <c r="E17" s="47"/>
+      <c r="F17" s="53" t="str">
+        <f t="shared" ref="F17:F19" si="7">+F16</f>
+        <v>Dcurso</v>
+      </c>
+      <c r="G17" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="I16" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="M16" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>Route::put('users/{users}',['uses' =&gt; 'UsersController@update','as'=&gt; 'admin.users.update']);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="C17" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v>users</v>
-      </c>
-      <c r="D17" s="64" t="str">
-        <f>+D16</f>
-        <v>users</v>
-      </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v>User</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="H17" s="28"/>
+      <c r="H17" s="28" t="s">
+        <v>313</v>
+      </c>
       <c r="I17" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="26" t="s">
-        <v>329</v>
+      <c r="J17" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L17" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>'dcursos/{dcursos}'</v>
       </c>
       <c r="M17" s="26" t="str">
+        <f t="shared" si="3"/>
+        <v>'uses'=&gt;'DcursosController@update'</v>
+      </c>
+      <c r="N17" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v>'as'=&gt;'admin.dcursos.update'</v>
+      </c>
+      <c r="O17" s="57" t="str">
         <f t="shared" si="1"/>
-        <v>Route::get('users/{users}',['uses' =&gt; 'UsersController@show','as'=&gt; 'admin.users.show']);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="51" t="s">
+        <v>Route::put('dcursos/{dcursos}',['uses'=&gt;'DcursosController@update','as'=&gt;'admin.dcursos.update']);</v>
+      </c>
+      <c r="P17" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::put('dcursos/{dcursos}',['uses' =&gt; 'DcursosController@update','as'=&gt; 'admin.dcursos.update']);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="53" t="str">
+        <f t="shared" si="6"/>
+        <v>dcursos</v>
+      </c>
+      <c r="D18" s="53" t="str">
+        <f>+D17</f>
+        <v>dcursos</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="53" t="str">
+        <f t="shared" si="7"/>
+        <v>Dcurso</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="H18" s="28"/>
+      <c r="I18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L18" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>'dcursos/{dcursos}'</v>
+      </c>
+      <c r="M18" s="26" t="str">
+        <f t="shared" si="3"/>
+        <v>'uses'=&gt;'DcursosController@show'</v>
+      </c>
+      <c r="N18" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v>'as'=&gt;'admin.dcursos.show'</v>
+      </c>
+      <c r="O18" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>Route::get('dcursos/{dcursos}',['uses'=&gt;'DcursosController@show','as'=&gt;'admin.dcursos.show']);</v>
+      </c>
+      <c r="P18" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::get('dcursos/{dcursos}',['uses' =&gt; 'DcursosController@show','as'=&gt; 'admin.dcursos.show']);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="42" t="s">
+        <v>324</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="53" t="str">
+        <f t="shared" si="6"/>
+        <v>dcursos</v>
+      </c>
+      <c r="D19" s="53" t="str">
+        <f>+D18</f>
+        <v>dcursos</v>
+      </c>
+      <c r="E19" s="48"/>
+      <c r="F19" s="53" t="str">
+        <f t="shared" si="7"/>
+        <v>Dcurso</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>admin.dcursos</v>
+      </c>
+      <c r="L19" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>'dcursos/{dcursos}'</v>
+      </c>
+      <c r="M19" s="26" t="str">
+        <f t="shared" si="3"/>
+        <v>'uses'=&gt;'DcursosController@destroy'</v>
+      </c>
+      <c r="N19" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v>'as'=&gt;'admin.dcursos.destroy'</v>
+      </c>
+      <c r="O19" s="57" t="str">
+        <f t="shared" si="1"/>
+        <v>Route::delete('dcursos/{dcursos}',['uses'=&gt;'DcursosController@destroy','as'=&gt;'admin.dcursos.destroy']);</v>
+      </c>
+      <c r="P19" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Route::delete('dcursos/{dcursos}',['uses' =&gt; 'DcursosController@destroy','as'=&gt; 'admin.dcursos.destroy']);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="55" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+    </row>
+    <row r="21" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="53" t="str">
+        <f>+G21</f>
+        <v>destroy</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>308</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="L21" s="26" t="str">
+        <f>+"'"&amp;C21&amp;IF(LEN(D21)&gt;0,"/{"&amp;D21&amp;"}","")&amp;IF(LEN(E21)&gt;0,"/"&amp;E21,"")&amp;"'"</f>
+        <v>'users/{id}/destroy'</v>
+      </c>
+      <c r="M21" s="26" t="str">
+        <f t="shared" ref="M21" si="8">+"'uses'=&gt;'"&amp;F21&amp;"sController@"&amp;G21&amp;"'"</f>
+        <v>'uses'=&gt;'UsersController@destroy'</v>
+      </c>
+      <c r="N21" s="26" t="str">
+        <f t="shared" ref="N21" si="9">+"'as'=&gt;'"&amp;J21&amp;"."&amp;G21&amp;"'"</f>
+        <v>'as'=&gt;'admin.users.destroy'</v>
+      </c>
+      <c r="O21" s="26" t="str">
+        <f>+"Route::"&amp;B21&amp;"("&amp;L21&amp;",["&amp;M21&amp;","&amp;N21&amp;"]);"</f>
+        <v>Route::get('users/{id}/destroy',['uses'=&gt;'UsersController@destroy','as'=&gt;'admin.users.destroy']);</v>
+      </c>
+      <c r="P21" s="26" t="str">
+        <f>+"Route::"&amp;B21&amp;"('"&amp;C21&amp;IF(LEN(D21)&gt;0,"/{"&amp;D21&amp;"}"&amp;IF(LEN(E21)&gt;0,"/"&amp;E21,""),"")&amp;"',['uses' =&gt; '"&amp;F21&amp;"sController@"&amp;G21&amp;"','as'=&gt; '"&amp;J21&amp;"."&amp;G21&amp;"']);"</f>
+        <v>Route::get('users/{id}/destroy',['uses' =&gt; 'UsersController@destroy','as'=&gt; 'admin.users.destroy']);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="26" t="s">
         <v>327</v>
-      </c>
-      <c r="B18" s="51" t="s">
-        <v>320</v>
-      </c>
-      <c r="C18" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>users</v>
-      </c>
-      <c r="D18" s="64" t="str">
-        <f>+D17</f>
-        <v>users</v>
-      </c>
-      <c r="E18" s="58"/>
-      <c r="F18" s="65" t="str">
-        <f t="shared" si="2"/>
-        <v>User</v>
-      </c>
-      <c r="G18" s="51" t="s">
-        <v>318</v>
-      </c>
-      <c r="H18" s="52"/>
-      <c r="I18" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" s="51" t="s">
-        <v>329</v>
-      </c>
-      <c r="M18" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>Route::delete('users/{users}',['uses' =&gt; 'UsersController@destroy','as'=&gt; 'admin.users.destroy']);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="26" t="s">
-        <v>328</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="C19" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v>users</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="26" t="str">
-        <f>+G19</f>
-        <v>destroy</v>
-      </c>
-      <c r="F19" s="64" t="str">
-        <f t="shared" si="2"/>
-        <v>User</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="M19" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>Route::get('users/{id}/destroy',['uses' =&gt; 'UsersController@destroy','as'=&gt; 'admin.users.destroy']);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="M21" s="26" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4007,6 +4702,7 @@
     <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4014,8 +4710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z192"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="N77" sqref="N77"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4040,22 +4736,22 @@
       <c r="A3" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="38">
         <v>11</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="38">
         <v>10</v>
       </c>
-      <c r="O3" s="43">
+      <c r="O3" s="38">
         <v>38</v>
       </c>
-      <c r="P3" s="43">
+      <c r="P3" s="38">
         <v>29</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="38">
         <v>65</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="38">
         <v>20</v>
       </c>
     </row>
@@ -4063,22 +4759,22 @@
       <c r="A4" t="s">
         <v>214</v>
       </c>
-      <c r="M4" s="43">
+      <c r="M4" s="38">
         <v>1</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="38">
         <v>1</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="38">
         <v>1</v>
       </c>
-      <c r="P4" s="43">
+      <c r="P4" s="38">
         <v>1</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="Q4" s="38">
         <v>1</v>
       </c>
-      <c r="R4" s="43">
+      <c r="R4" s="38">
         <v>1</v>
       </c>
     </row>
@@ -4086,19 +4782,19 @@
       <c r="A5" t="s">
         <v>211</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -7480,20 +8176,20 @@
       </c>
     </row>
     <row r="153" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="42" t="s">
+      <c r="A153" s="37" t="s">
         <v>286</v>
       </c>
-      <c r="B153" s="42"/>
-      <c r="C153" s="42"/>
-      <c r="D153" s="42"/>
-      <c r="E153" s="42"/>
-      <c r="F153" s="42"/>
-      <c r="G153" s="42"/>
-      <c r="H153" s="42"/>
-      <c r="I153" s="42"/>
-      <c r="J153" s="42"/>
-      <c r="K153" s="42"/>
-      <c r="L153" s="42"/>
+      <c r="B153" s="37"/>
+      <c r="C153" s="37"/>
+      <c r="D153" s="37"/>
+      <c r="E153" s="37"/>
+      <c r="F153" s="37"/>
+      <c r="G153" s="37"/>
+      <c r="H153" s="37"/>
+      <c r="I153" s="37"/>
+      <c r="J153" s="37"/>
+      <c r="K153" s="37"/>
+      <c r="L153" s="37"/>
       <c r="N153" t="str">
         <f>MID($A153,SUM($L$3:M$4),N$3)</f>
         <v xml:space="preserve">GET|HEAD  </v>
@@ -7516,9 +8212,21 @@
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+      <c r="A154" s="34" t="s">
         <v>216</v>
       </c>
+      <c r="B154" s="34"/>
+      <c r="C154" s="34"/>
+      <c r="D154" s="34"/>
+      <c r="E154" s="34"/>
+      <c r="F154" s="34"/>
+      <c r="G154" s="34"/>
+      <c r="H154" s="34"/>
+      <c r="I154" s="34"/>
+      <c r="J154" s="34"/>
+      <c r="K154" s="34"/>
+      <c r="L154" s="34"/>
+      <c r="M154" s="34"/>
       <c r="N154" t="str">
         <f>MID($A154,SUM($L$3:M$4),N$3)</f>
         <v/>
@@ -7541,9 +8249,21 @@
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+      <c r="A155" s="34" t="s">
         <v>290</v>
       </c>
+      <c r="B155" s="34"/>
+      <c r="C155" s="34"/>
+      <c r="D155" s="34"/>
+      <c r="E155" s="34"/>
+      <c r="F155" s="34"/>
+      <c r="G155" s="34"/>
+      <c r="H155" s="34"/>
+      <c r="I155" s="34"/>
+      <c r="J155" s="34"/>
+      <c r="K155" s="34"/>
+      <c r="L155" s="34"/>
+      <c r="M155" s="34"/>
       <c r="N155" t="str">
         <f>MID($A155,SUM($L$3:M$4),N$3)</f>
         <v xml:space="preserve">GET|HEAD  </v>

</xml_diff>

<commit_message>
Version 1.01 con instrucciones
</commit_message>
<xml_diff>
--- a/topdown/topdown FCEC.xlsx
+++ b/topdown/topdown FCEC.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="403">
   <si>
     <t>NOMBRE DEL PROYECTO:</t>
   </si>
@@ -886,27 +886,6 @@
     <t>todo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/update</t>
-    </r>
-  </si>
-  <si>
     <t>+--------+-----------+--------------------------------------+-----------------------------+-----------------------------------------------------------------+---------------</t>
   </si>
   <si>
@@ -1475,6 +1454,15 @@
   </si>
   <si>
     <t>https://styde.net/sistema-de-archivos-y-almacenamiento-en-laravel-5/</t>
+  </si>
+  <si>
+    <t>CARGA ASIGNADA</t>
+  </si>
+  <si>
+    <t>Estructura de datos</t>
+  </si>
+  <si>
+    <t>Correo de comunicación</t>
   </si>
 </sst>
 </file>
@@ -2188,10 +2176,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2259,7 +2247,7 @@
         <v>75</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2270,7 +2258,7 @@
         <v>188</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H5" s="30"/>
     </row>
@@ -2359,18 +2347,16 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B14" s="27" t="s">
+    <row r="14" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="33"/>
+      <c r="B14" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>210</v>
+      <c r="D14" s="22" t="s">
+        <v>189</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>197</v>
@@ -2391,11 +2377,14 @@
         <v>192</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="32" t="s">
+        <v>185</v>
+      </c>
       <c r="B17" s="10" t="s">
         <v>172</v>
       </c>
@@ -2590,23 +2579,23 @@
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="F37" s="31" t="s">
         <v>392</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -2614,10 +2603,10 @@
         <v>185</v>
       </c>
       <c r="B38" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="F38" s="27" t="s">
         <v>394</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2625,10 +2614,10 @@
         <v>185</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2636,12 +2625,12 @@
         <v>185</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B42" s="26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -2649,10 +2638,42 @@
         <v>185</v>
       </c>
       <c r="B43" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="F43" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="F43" s="27" t="s">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" s="26" t="s">
         <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -2684,142 +2705,142 @@
   <sheetData>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
@@ -2829,197 +2850,197 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4266,7 +4287,7 @@
     </row>
     <row r="9" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -4280,65 +4301,65 @@
     <row r="10" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="35"/>
       <c r="C10" s="64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="66"/>
       <c r="F10" s="67" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G10" s="68"/>
       <c r="H10" s="68"/>
       <c r="I10" s="69"/>
       <c r="J10" s="35"/>
       <c r="L10" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="M10" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="M10" s="26" t="s">
-        <v>342</v>
-      </c>
       <c r="O10" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="H11" s="39" t="s">
         <v>331</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>334</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>338</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>329</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>330</v>
-      </c>
-      <c r="H11" s="39" t="s">
+      <c r="I11" s="40" t="s">
         <v>332</v>
       </c>
-      <c r="I11" s="40" t="s">
-        <v>333</v>
-      </c>
       <c r="J11" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M11" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="N11" s="26" t="s">
         <v>343</v>
-      </c>
-      <c r="N11" s="26" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="52" t="str">
@@ -4351,7 +4372,7 @@
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="46"/>
@@ -4359,10 +4380,10 @@
     </row>
     <row r="13" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C13" s="53" t="str">
         <f>+C12</f>
@@ -4378,7 +4399,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J13" s="26" t="str">
         <f>+"admin."&amp;$D$12</f>
@@ -4407,10 +4428,10 @@
     </row>
     <row r="14" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C14" s="53" t="str">
         <f>+C15</f>
@@ -4456,10 +4477,10 @@
     </row>
     <row r="15" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C15" s="53" t="str">
         <f>+C13</f>
@@ -4472,10 +4493,10 @@
         <v>Dcurso</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J15" s="26" t="str">
         <f t="shared" ref="J15:J19" si="5">+J14</f>
@@ -4504,10 +4525,10 @@
     </row>
     <row r="16" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C16" s="53" t="str">
         <f>+C14</f>
@@ -4554,10 +4575,10 @@
     </row>
     <row r="17" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C17" s="53" t="str">
         <f t="shared" ref="C17:C19" si="6">+C16</f>
@@ -4573,10 +4594,10 @@
         <v>Dcurso</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I17" s="26" t="s">
         <v>35</v>
@@ -4608,10 +4629,10 @@
     </row>
     <row r="18" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C18" s="53" t="str">
         <f t="shared" si="6"/>
@@ -4627,7 +4648,7 @@
         <v>Dcurso</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="26" t="s">
@@ -4660,10 +4681,10 @@
     </row>
     <row r="19" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C19" s="53" t="str">
         <f t="shared" si="6"/>
@@ -4679,7 +4700,7 @@
         <v>Dcurso</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H19" s="43"/>
       <c r="I19" s="42" t="s">
@@ -4723,10 +4744,10 @@
     </row>
     <row r="21" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C21" s="53" t="s">
         <v>26</v>
@@ -4739,17 +4760,17 @@
         <v>destroy</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="26" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L21" s="26" t="str">
         <f>+"'"&amp;C21&amp;IF(LEN(D21)&gt;0,"/{"&amp;D21&amp;"}","")&amp;IF(LEN(E21)&gt;0,"/"&amp;E21,"")&amp;"'"</f>
@@ -4774,7 +4795,7 @@
     </row>
     <row r="23" spans="1:16" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L23" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4805,17 +4826,17 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M3" s="38">
         <v>11</v>
@@ -4838,7 +4859,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M4" s="38">
         <v>1</v>
@@ -4861,7 +4882,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
@@ -4879,22 +4900,22 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M9" t="str">
         <f>LEFT($A9,M$3)</f>
@@ -4923,12 +4944,12 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N11" t="str">
         <f>MID($A11,SUM($L$3:M$4),N$3)</f>
@@ -4953,12 +4974,12 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N13" t="str">
         <f>MID($A13,SUM($L$3:M$4),N$3)</f>
@@ -4983,12 +5004,12 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N15" t="str">
         <f>MID($A15,SUM($L$3:M$4),N$3)</f>
@@ -5013,12 +5034,12 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N17" t="str">
         <f>MID($A17,SUM($L$3:M$4),N$3)</f>
@@ -5043,12 +5064,12 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N19" t="str">
         <f>MID($A19,SUM($L$3:M$4),N$3)</f>
@@ -5073,12 +5094,12 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N21" t="str">
         <f>MID($A21,SUM($L$3:M$4),N$3)</f>
@@ -5103,12 +5124,12 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N23" t="str">
         <f>MID($A23,SUM($L$3:M$4),N$3)</f>
@@ -5133,12 +5154,12 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N25" t="str">
         <f>MID($A25,SUM($L$3:M$4),N$3)</f>
@@ -5163,12 +5184,12 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N27" t="str">
         <f>MID($A27,SUM($L$3:M$4),N$3)</f>
@@ -5193,12 +5214,12 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N29" t="str">
         <f>MID($A29,SUM($L$3:M$4),N$3)</f>
@@ -5223,12 +5244,12 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N31" t="str">
         <f>MID($A31,SUM($L$3:M$4),N$3)</f>
@@ -5253,12 +5274,12 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N33" t="str">
         <f>MID($A33,SUM($L$3:M$4),N$3)</f>
@@ -5283,7 +5304,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N34" t="str">
         <f>MID($A34,SUM($L$3:M$4),N$3)</f>
@@ -5308,7 +5329,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N35" t="str">
         <f>MID($A35,SUM($L$3:M$4),N$3)</f>
@@ -5333,7 +5354,7 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N36" t="str">
         <f>MID($A36,SUM($L$3:M$4),N$3)</f>
@@ -5358,7 +5379,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N37" t="str">
         <f>MID($A37,SUM($L$3:M$4),N$3)</f>
@@ -5383,7 +5404,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N38" t="str">
         <f>MID($A38,SUM($L$3:M$4),N$3)</f>
@@ -5408,7 +5429,7 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N39" t="str">
         <f>MID($A39,SUM($L$3:M$4),N$3)</f>
@@ -5433,7 +5454,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N40" t="str">
         <f>MID($A40,SUM($L$3:M$4),N$3)</f>
@@ -5458,7 +5479,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N41" t="str">
         <f>MID($A41,SUM($L$3:M$4),N$3)</f>
@@ -5483,7 +5504,7 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N42" t="str">
         <f>MID($A42,SUM($L$3:M$4),N$3)</f>
@@ -5508,7 +5529,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N43" t="str">
         <f>MID($A43,SUM($L$3:M$4),N$3)</f>
@@ -5533,7 +5554,7 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N44" t="str">
         <f>MID($A44,SUM($L$3:M$4),N$3)</f>
@@ -5558,7 +5579,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N45" t="str">
         <f>MID($A45,SUM($L$3:M$4),N$3)</f>
@@ -5583,7 +5604,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N46" t="str">
         <f>MID($A46,SUM($L$3:M$4),N$3)</f>
@@ -5608,7 +5629,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N47" t="str">
         <f>MID($A47,SUM($L$3:M$4),N$3)</f>
@@ -5633,7 +5654,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N48" t="str">
         <f>MID($A48,SUM($L$3:M$4),N$3)</f>
@@ -5658,7 +5679,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N49" t="str">
         <f>MID($A49,SUM($L$3:M$4),N$3)</f>
@@ -5683,7 +5704,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N50" t="str">
         <f>MID($A50,SUM($L$3:M$4),N$3)</f>
@@ -5708,7 +5729,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N51" t="str">
         <f>MID($A51,SUM($L$3:M$4),N$3)</f>
@@ -5733,7 +5754,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N52" t="str">
         <f>MID($A52,SUM($L$3:M$4),N$3)</f>
@@ -5758,7 +5779,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N53" t="str">
         <f>MID($A53,SUM($L$3:M$4),N$3)</f>
@@ -5783,7 +5804,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N54" t="str">
         <f>MID($A54,SUM($L$3:M$4),N$3)</f>
@@ -5808,7 +5829,7 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N55" t="str">
         <f>MID($A55,SUM($L$3:M$4),N$3)</f>
@@ -5833,7 +5854,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N56" t="str">
         <f>MID($A56,SUM($L$3:M$4),N$3)</f>
@@ -5858,7 +5879,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N57" t="str">
         <f>MID($A57,SUM($L$3:M$4),N$3)</f>
@@ -5883,7 +5904,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N58" t="str">
         <f>MID($A58,SUM($L$3:M$4),N$3)</f>
@@ -5908,7 +5929,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N59" t="str">
         <f>MID($A59,SUM($L$3:M$4),N$3)</f>
@@ -5933,7 +5954,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N60" t="str">
         <f>MID($A60,SUM($L$3:M$4),N$3)</f>
@@ -5958,7 +5979,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N61" t="str">
         <f>MID($A61,SUM($L$3:M$4),N$3)</f>
@@ -5983,7 +6004,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N62" t="str">
         <f>MID($A62,SUM($L$3:M$4),N$3)</f>
@@ -6008,7 +6029,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N63" t="str">
         <f>MID($A63,SUM($L$3:M$4),N$3)</f>
@@ -6033,7 +6054,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N64" t="str">
         <f>MID($A64,SUM($L$3:M$4),N$3)</f>
@@ -6058,7 +6079,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N65" t="str">
         <f>MID($A65,SUM($L$3:M$4),N$3)</f>
@@ -6083,7 +6104,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N66" t="str">
         <f>MID($A66,SUM($L$3:M$4),N$3)</f>
@@ -6108,7 +6129,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N67" t="str">
         <f>MID($A67,SUM($L$3:M$4),N$3)</f>
@@ -6133,7 +6154,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N68" t="str">
         <f>MID($A68,SUM($L$3:M$4),N$3)</f>
@@ -6158,7 +6179,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N69" t="str">
         <f>MID($A69,SUM($L$3:M$4),N$3)</f>
@@ -6183,7 +6204,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N70" t="str">
         <f>MID($A70,SUM($L$3:M$4),N$3)</f>
@@ -6208,7 +6229,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N71" t="str">
         <f>MID($A71,SUM($L$3:M$4),N$3)</f>
@@ -6233,7 +6254,7 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N72" t="str">
         <f>MID($A72,SUM($L$3:M$4),N$3)</f>
@@ -6258,7 +6279,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N73" t="str">
         <f>MID($A73,SUM($L$3:M$4),N$3)</f>
@@ -6283,7 +6304,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N74" t="str">
         <f>MID($A74,SUM($L$3:M$4),N$3)</f>
@@ -6308,7 +6329,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N75" t="str">
         <f>MID($A75,SUM($L$3:M$4),N$3)</f>
@@ -6333,7 +6354,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N76" t="str">
         <f>MID($A76,SUM($L$3:M$4),N$3)</f>
@@ -6358,7 +6379,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N77" t="str">
         <f>MID($A77,SUM($L$3:M$4),N$3)</f>
@@ -6383,7 +6404,7 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N78" t="str">
         <f>MID($A78,SUM($L$3:M$4),N$3)</f>
@@ -6408,7 +6429,7 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N79" t="str">
         <f>MID($A79,SUM($L$3:M$4),N$3)</f>
@@ -6433,7 +6454,7 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N80" t="str">
         <f>MID($A80,SUM($L$3:M$4),N$3)</f>
@@ -6458,7 +6479,7 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N81" t="str">
         <f>MID($A81,SUM($L$3:M$4),N$3)</f>
@@ -6483,7 +6504,7 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N82" t="str">
         <f>MID($A82,SUM($L$3:M$4),N$3)</f>
@@ -6508,7 +6529,7 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N83" t="str">
         <f>MID($A83,SUM($L$3:M$4),N$3)</f>
@@ -6533,7 +6554,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N84" t="str">
         <f>MID($A84,SUM($L$3:M$4),N$3)</f>
@@ -6558,7 +6579,7 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N85" t="str">
         <f>MID($A85,SUM($L$3:M$4),N$3)</f>
@@ -6583,7 +6604,7 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N86" t="str">
         <f>MID($A86,SUM($L$3:M$4),N$3)</f>
@@ -6608,7 +6629,7 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N87" t="str">
         <f>MID($A87,SUM($L$3:M$4),N$3)</f>
@@ -6633,7 +6654,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N88" t="str">
         <f>MID($A88,SUM($L$3:M$4),N$3)</f>
@@ -6658,7 +6679,7 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N89" t="str">
         <f>MID($A89,SUM($L$3:M$4),N$3)</f>
@@ -6683,7 +6704,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N90" t="str">
         <f>MID($A90,SUM($L$3:M$4),N$3)</f>
@@ -6708,7 +6729,7 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N91" t="str">
         <f>MID($A91,SUM($L$3:M$4),N$3)</f>
@@ -6733,7 +6754,7 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N92" t="str">
         <f>MID($A92,SUM($L$3:M$4),N$3)</f>
@@ -6758,7 +6779,7 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N93" t="str">
         <f>MID($A93,SUM($L$3:M$4),N$3)</f>
@@ -6783,7 +6804,7 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N94" t="str">
         <f>MID($A94,SUM($L$3:M$4),N$3)</f>
@@ -6808,7 +6829,7 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N95" t="str">
         <f>MID($A95,SUM($L$3:M$4),N$3)</f>
@@ -6833,7 +6854,7 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N96" t="str">
         <f>MID($A96,SUM($L$3:M$4),N$3)</f>
@@ -6858,7 +6879,7 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N97" t="str">
         <f>MID($A97,SUM($L$3:M$4),N$3)</f>
@@ -6883,7 +6904,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N98" t="str">
         <f>MID($A98,SUM($L$3:M$4),N$3)</f>
@@ -6908,7 +6929,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N99" t="str">
         <f>MID($A99,SUM($L$3:M$4),N$3)</f>
@@ -6933,7 +6954,7 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N100" t="str">
         <f>MID($A100,SUM($L$3:M$4),N$3)</f>
@@ -6958,7 +6979,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N101" t="str">
         <f>MID($A101,SUM($L$3:M$4),N$3)</f>
@@ -6983,7 +7004,7 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N102" t="str">
         <f>MID($A102,SUM($L$3:M$4),N$3)</f>
@@ -7008,7 +7029,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N103" t="str">
         <f>MID($A103,SUM($L$3:M$4),N$3)</f>
@@ -7033,7 +7054,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N104" t="str">
         <f>MID($A104,SUM($L$3:M$4),N$3)</f>
@@ -7058,7 +7079,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N105" t="str">
         <f>MID($A105,SUM($L$3:M$4),N$3)</f>
@@ -7083,7 +7104,7 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N106" t="str">
         <f>MID($A106,SUM($L$3:M$4),N$3)</f>
@@ -7108,7 +7129,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N107" t="str">
         <f>MID($A107,SUM($L$3:M$4),N$3)</f>
@@ -7133,7 +7154,7 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N108" t="str">
         <f>MID($A108,SUM($L$3:M$4),N$3)</f>
@@ -7158,7 +7179,7 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N109" t="str">
         <f>MID($A109,SUM($L$3:M$4),N$3)</f>
@@ -7183,7 +7204,7 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N110" t="str">
         <f>MID($A110,SUM($L$3:M$4),N$3)</f>
@@ -7208,7 +7229,7 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N111" t="str">
         <f>MID($A111,SUM($L$3:M$4),N$3)</f>
@@ -7233,7 +7254,7 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N112" t="str">
         <f>MID($A112,SUM($L$3:M$4),N$3)</f>
@@ -7258,7 +7279,7 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N113" t="str">
         <f>MID($A113,SUM($L$3:M$4),N$3)</f>
@@ -7283,7 +7304,7 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N114" t="str">
         <f>MID($A114,SUM($L$3:M$4),N$3)</f>
@@ -7308,7 +7329,7 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N115" t="str">
         <f>MID($A115,SUM($L$3:M$4),N$3)</f>
@@ -7333,7 +7354,7 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N116" t="str">
         <f>MID($A116,SUM($L$3:M$4),N$3)</f>
@@ -7358,7 +7379,7 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N117" t="str">
         <f>MID($A117,SUM($L$3:M$4),N$3)</f>
@@ -7383,7 +7404,7 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N118" t="str">
         <f>MID($A118,SUM($L$3:M$4),N$3)</f>
@@ -7408,7 +7429,7 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N119" t="str">
         <f>MID($A119,SUM($L$3:M$4),N$3)</f>
@@ -7433,7 +7454,7 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N120" t="str">
         <f>MID($A120,SUM($L$3:M$4),N$3)</f>
@@ -7458,7 +7479,7 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N121" t="str">
         <f>MID($A121,SUM($L$3:M$4),N$3)</f>
@@ -7483,7 +7504,7 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N122" t="str">
         <f>MID($A122,SUM($L$3:M$4),N$3)</f>
@@ -7508,7 +7529,7 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N123" t="str">
         <f>MID($A123,SUM($L$3:M$4),N$3)</f>
@@ -7533,7 +7554,7 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N124" t="str">
         <f>MID($A124,SUM($L$3:M$4),N$3)</f>
@@ -7558,7 +7579,7 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N125" t="str">
         <f>MID($A125,SUM($L$3:M$4),N$3)</f>
@@ -7583,7 +7604,7 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N126" t="str">
         <f>MID($A126,SUM($L$3:M$4),N$3)</f>
@@ -7608,7 +7629,7 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N127" t="str">
         <f>MID($A127,SUM($L$3:M$4),N$3)</f>
@@ -7633,7 +7654,7 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N128" t="str">
         <f>MID($A128,SUM($L$3:M$4),N$3)</f>
@@ -7658,7 +7679,7 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N129" t="str">
         <f>MID($A129,SUM($L$3:M$4),N$3)</f>
@@ -7683,7 +7704,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N130" t="str">
         <f>MID($A130,SUM($L$3:M$4),N$3)</f>
@@ -7708,7 +7729,7 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N131" t="str">
         <f>MID($A131,SUM($L$3:M$4),N$3)</f>
@@ -7733,7 +7754,7 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N132" t="str">
         <f>MID($A132,SUM($L$3:M$4),N$3)</f>
@@ -7758,7 +7779,7 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N133" t="str">
         <f>MID($A133,SUM($L$3:M$4),N$3)</f>
@@ -7783,7 +7804,7 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N134" t="str">
         <f>MID($A134,SUM($L$3:M$4),N$3)</f>
@@ -7808,7 +7829,7 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N135" t="str">
         <f>MID($A135,SUM($L$3:M$4),N$3)</f>
@@ -7833,7 +7854,7 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N136" t="str">
         <f>MID($A136,SUM($L$3:M$4),N$3)</f>
@@ -7858,7 +7879,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N137" t="str">
         <f>MID($A137,SUM($L$3:M$4),N$3)</f>
@@ -7883,7 +7904,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N138" t="str">
         <f>MID($A138,SUM($L$3:M$4),N$3)</f>
@@ -7908,7 +7929,7 @@
     </row>
     <row r="139" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N139" t="str">
         <f>MID($A139,SUM($L$3:M$4),N$3)</f>
@@ -7933,7 +7954,7 @@
     </row>
     <row r="140" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N140" t="str">
         <f>MID($A140,SUM($L$3:M$4),N$3)</f>
@@ -7958,7 +7979,7 @@
     </row>
     <row r="141" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N141" t="str">
         <f>MID($A141,SUM($L$3:M$4),N$3)</f>
@@ -7983,7 +8004,7 @@
     </row>
     <row r="142" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N142" t="str">
         <f>MID($A142,SUM($L$3:M$4),N$3)</f>
@@ -8008,7 +8029,7 @@
     </row>
     <row r="143" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N143" t="str">
         <f>MID($A143,SUM($L$3:M$4),N$3)</f>
@@ -8033,7 +8054,7 @@
     </row>
     <row r="144" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A144" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N144" t="str">
         <f>MID($A144,SUM($L$3:M$4),N$3)</f>
@@ -8058,7 +8079,7 @@
     </row>
     <row r="145" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N145" t="str">
         <f>MID($A145,SUM($L$3:M$4),N$3)</f>
@@ -8083,7 +8104,7 @@
     </row>
     <row r="146" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N146" t="str">
         <f>MID($A146,SUM($L$3:M$4),N$3)</f>
@@ -8108,7 +8129,7 @@
     </row>
     <row r="147" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N147" t="str">
         <f>MID($A147,SUM($L$3:M$4),N$3)</f>
@@ -8133,7 +8154,7 @@
     </row>
     <row r="148" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N148" t="str">
         <f>MID($A148,SUM($L$3:M$4),N$3)</f>
@@ -8158,7 +8179,7 @@
     </row>
     <row r="149" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N149" t="str">
         <f>MID($A149,SUM($L$3:M$4),N$3)</f>
@@ -8183,7 +8204,7 @@
     </row>
     <row r="150" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N150" t="str">
         <f>MID($A150,SUM($L$3:M$4),N$3)</f>
@@ -8208,7 +8229,7 @@
     </row>
     <row r="151" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N151" t="str">
         <f>MID($A151,SUM($L$3:M$4),N$3)</f>
@@ -8233,7 +8254,7 @@
     </row>
     <row r="152" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N152" t="str">
         <f>MID($A152,SUM($L$3:M$4),N$3)</f>
@@ -8258,7 +8279,7 @@
     </row>
     <row r="153" spans="1:18" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B153" s="37"/>
       <c r="C153" s="37"/>
@@ -8294,7 +8315,7 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B154" s="34"/>
       <c r="C154" s="34"/>
@@ -8331,7 +8352,7 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A155" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B155" s="34"/>
       <c r="C155" s="34"/>
@@ -8368,7 +8389,7 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N156" t="str">
         <f>MID($A156,SUM($L$3:M$4),N$3)</f>
@@ -8393,7 +8414,7 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N157" t="str">
         <f>MID($A157,SUM($L$3:M$4),N$3)</f>
@@ -8418,7 +8439,7 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N158" t="str">
         <f>MID($A158,SUM($L$3:M$4),N$3)</f>
@@ -8443,7 +8464,7 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N159" t="str">
         <f>MID($A159,SUM($L$3:M$4),N$3)</f>
@@ -8468,7 +8489,7 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N160" t="str">
         <f>MID($A160,SUM($L$3:M$4),N$3)</f>
@@ -8493,7 +8514,7 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N161" t="str">
         <f>MID($A161,SUM($L$3:M$4),N$3)</f>
@@ -8518,7 +8539,7 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N162" t="str">
         <f>MID($A162,SUM($L$3:M$4),N$3)</f>
@@ -8543,7 +8564,7 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N163" t="str">
         <f>MID($A163,SUM($L$3:M$4),N$3)</f>
@@ -8568,7 +8589,7 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N164" t="str">
         <f>MID($A164,SUM($L$3:M$4),N$3)</f>
@@ -8593,7 +8614,7 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N165" t="str">
         <f>MID($A165,SUM($L$3:M$4),N$3)</f>
@@ -8618,7 +8639,7 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N166" t="str">
         <f>MID($A166,SUM($L$3:M$4),N$3)</f>
@@ -8643,7 +8664,7 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N167" t="str">
         <f>MID($A167,SUM($L$3:M$4),N$3)</f>
@@ -8668,7 +8689,7 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N168" t="str">
         <f>MID($A168,SUM($L$3:M$4),N$3)</f>
@@ -8693,7 +8714,7 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N169" t="str">
         <f>MID($A169,SUM($L$3:M$4),N$3)</f>
@@ -8718,7 +8739,7 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N170" t="str">
         <f>MID($A170,SUM($L$3:M$4),N$3)</f>
@@ -8743,7 +8764,7 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N171" t="str">
         <f>MID($A171,SUM($L$3:M$4),N$3)</f>
@@ -8768,7 +8789,7 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N172" t="str">
         <f>MID($A172,SUM($L$3:M$4),N$3)</f>
@@ -8793,7 +8814,7 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N173" t="str">
         <f>MID($A173,SUM($L$3:M$4),N$3)</f>
@@ -8818,7 +8839,7 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N174" t="str">
         <f>MID($A174,SUM($L$3:M$4),N$3)</f>
@@ -8843,7 +8864,7 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N175" t="str">
         <f>MID($A175,SUM($L$3:M$4),N$3)</f>
@@ -8868,7 +8889,7 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N176" t="str">
         <f>MID($A176,SUM($L$3:M$4),N$3)</f>
@@ -8893,7 +8914,7 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N177" t="str">
         <f>MID($A177,SUM($L$3:M$4),N$3)</f>
@@ -8918,7 +8939,7 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N178" t="str">
         <f>MID($A178,SUM($L$3:M$4),N$3)</f>
@@ -8943,7 +8964,7 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N179" t="str">
         <f>MID($A179,SUM($L$3:M$4),N$3)</f>
@@ -8968,7 +8989,7 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N180" t="str">
         <f>MID($A180,SUM($L$3:M$4),N$3)</f>
@@ -8993,7 +9014,7 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N181" t="str">
         <f>MID($A181,SUM($L$3:M$4),N$3)</f>
@@ -9018,7 +9039,7 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N182" t="str">
         <f>MID($A182,SUM($L$3:M$4),N$3)</f>
@@ -9043,7 +9064,7 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N183" t="str">
         <f>MID($A183,SUM($L$3:M$4),N$3)</f>
@@ -9068,7 +9089,7 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N184" t="str">
         <f>MID($A184,SUM($L$3:M$4),N$3)</f>
@@ -9093,7 +9114,7 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N185" t="str">
         <f>MID($A185,SUM($L$3:M$4),N$3)</f>
@@ -9118,7 +9139,7 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N186" t="str">
         <f>MID($A186,SUM($L$3:M$4),N$3)</f>
@@ -9143,7 +9164,7 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N187" t="str">
         <f>MID($A187,SUM($L$3:M$4),N$3)</f>
@@ -9168,7 +9189,7 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N188" t="str">
         <f>MID($A188,SUM($L$3:M$4),N$3)</f>
@@ -9193,7 +9214,7 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N189" t="str">
         <f>MID($A189,SUM($L$3:M$4),N$3)</f>
@@ -9218,7 +9239,7 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N190" t="str">
         <f>MID($A190,SUM($L$3:M$4),N$3)</f>
@@ -9243,12 +9264,12 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>